<commit_message>
Added percentage error calculation
</commit_message>
<xml_diff>
--- a/docs/testing.xlsx
+++ b/docs/testing.xlsx
@@ -1,39 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>Note</t>
   </si>
   <si>
-    <t xml:space="preserve">MIDI #</t>
+    <t>MIDI #</t>
   </si>
   <si>
     <t>Frequency</t>
   </si>
   <si>
-    <t xml:space="preserve">Measured PWM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Measured audio freq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PWM diff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">audio diff</t>
+    <t>Measured PWM</t>
+  </si>
+  <si>
+    <t>Measured audio freq</t>
+  </si>
+  <si>
+    <t>PWM diff</t>
+  </si>
+  <si>
+    <t>audio diff</t>
   </si>
   <si>
     <t xml:space="preserve"> A0</t>
@@ -81,7 +82,7 @@
     <t xml:space="preserve"> B1</t>
   </si>
   <si>
-    <t xml:space="preserve">Not easily detectable at such low ranges</t>
+    <t>Not easily detectable at such low ranges</t>
   </si>
   <si>
     <t xml:space="preserve"> C2</t>
@@ -301,24 +302,39 @@
   </si>
   <si>
     <t xml:space="preserve"> C8</t>
+  </si>
+  <si>
+    <t>PWM delta</t>
+  </si>
+  <si>
+    <t>audio delta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <b/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <sz val="12"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -330,7 +346,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -578,78 +594,106 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="27">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="10" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="11" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="13" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="13" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="14" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="16" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -661,291 +705,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <a:themeElements>
     <a:clrScheme name="">
       <a:dk1>
@@ -997,7 +758,7 @@
         <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1068,30 +829,34 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
-      <pane state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="1" style="1" width="10.28125"/>
-    <col bestFit="1" customWidth="1" min="2" max="2" style="1" width="7.8515625"/>
-    <col bestFit="1" customWidth="1" min="3" max="3" style="1" width="14.00390625"/>
-    <col bestFit="1" customWidth="1" min="4" max="4" style="1" width="21.28125"/>
-    <col bestFit="1" customWidth="1" min="5" max="5" style="1" width="23.57421875"/>
-    <col bestFit="1" customWidth="1" min="6" max="6" style="1" width="12.140625"/>
-    <col bestFit="1" customWidth="1" min="7" max="7" style="1" width="10.00390625"/>
-    <col bestFit="1" min="8" max="16384" style="1" width="9.140625"/>
+    <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5">
+    <row r="1" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1113,8 +878,14 @@
       <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="H1" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -1127,15 +898,23 @@
       <c r="D2" s="8"/>
       <c r="E2" s="9"/>
       <c r="F2" s="10">
-        <f>ABS(C2-D2)</f>
+        <f t="shared" ref="F2:F33" si="0">ABS(C2-D2)</f>
         <v>27.5</v>
       </c>
       <c r="G2" s="11">
-        <f>ABS(C2-E2)</f>
+        <f t="shared" ref="G2:G33" si="1">ABS(C2-E2)</f>
         <v>27.5</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="H2" s="22" t="e">
+        <f>F2/D2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I2" s="24" t="e">
+        <f>G2/E2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>8</v>
       </c>
@@ -1148,15 +927,23 @@
       <c r="D3" s="13"/>
       <c r="E3" s="14"/>
       <c r="F3" s="10">
-        <f>ABS(C3-D3)</f>
+        <f t="shared" si="0"/>
         <v>29.135000000000002</v>
       </c>
       <c r="G3" s="11">
-        <f>ABS(C3-E3)</f>
+        <f t="shared" si="1"/>
         <v>29.135000000000002</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="H3" s="22" t="e">
+        <f t="shared" ref="H3:H66" si="2">F3/D3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I3" s="25" t="e">
+        <f t="shared" ref="I3:I66" si="3">G3/E3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>9</v>
       </c>
@@ -1169,15 +956,23 @@
       <c r="D4" s="13"/>
       <c r="E4" s="14"/>
       <c r="F4" s="10">
-        <f>ABS(C4-D4)</f>
+        <f t="shared" si="0"/>
         <v>30.867999999999999</v>
       </c>
       <c r="G4" s="11">
-        <f>ABS(C4-E4)</f>
+        <f t="shared" si="1"/>
         <v>30.867999999999999</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="H4" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I4" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>10</v>
       </c>
@@ -1190,15 +985,23 @@
       <c r="D5" s="13"/>
       <c r="E5" s="14"/>
       <c r="F5" s="10">
-        <f>ABS(C5-D5)</f>
+        <f t="shared" si="0"/>
         <v>32.703000000000003</v>
       </c>
       <c r="G5" s="11">
-        <f>ABS(C5-E5)</f>
+        <f t="shared" si="1"/>
         <v>32.703000000000003</v>
       </c>
-    </row>
-    <row r="6">
+      <c r="H5" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I5" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>11</v>
       </c>
@@ -1211,15 +1014,23 @@
       <c r="D6" s="13"/>
       <c r="E6" s="14"/>
       <c r="F6" s="10">
-        <f>ABS(C6-D6)</f>
+        <f t="shared" si="0"/>
         <v>34.683999999999997</v>
       </c>
       <c r="G6" s="11">
-        <f>ABS(C6-E6)</f>
+        <f t="shared" si="1"/>
         <v>34.683999999999997</v>
       </c>
-    </row>
-    <row r="7">
+      <c r="H6" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I6" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>12</v>
       </c>
@@ -1232,15 +1043,23 @@
       <c r="D7" s="13"/>
       <c r="E7" s="14"/>
       <c r="F7" s="10">
-        <f>ABS(C7-D7)</f>
+        <f t="shared" si="0"/>
         <v>36.707999999999998</v>
       </c>
       <c r="G7" s="11">
-        <f>ABS(C7-E7)</f>
+        <f t="shared" si="1"/>
         <v>36.707999999999998</v>
       </c>
-    </row>
-    <row r="8">
+      <c r="H7" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I7" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>13</v>
       </c>
@@ -1253,15 +1072,23 @@
       <c r="D8" s="13"/>
       <c r="E8" s="14"/>
       <c r="F8" s="10">
-        <f>ABS(C8-D8)</f>
+        <f t="shared" si="0"/>
         <v>38.890999999999998</v>
       </c>
       <c r="G8" s="11">
-        <f>ABS(C8-E8)</f>
+        <f t="shared" si="1"/>
         <v>38.890999999999998</v>
       </c>
-    </row>
-    <row r="9">
+      <c r="H8" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I8" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>14</v>
       </c>
@@ -1274,15 +1101,23 @@
       <c r="D9" s="13"/>
       <c r="E9" s="14"/>
       <c r="F9" s="10">
-        <f>ABS(C9-D9)</f>
+        <f t="shared" si="0"/>
         <v>41.203000000000003</v>
       </c>
       <c r="G9" s="11">
-        <f>ABS(C9-E9)</f>
+        <f t="shared" si="1"/>
         <v>41.203000000000003</v>
       </c>
-    </row>
-    <row r="10">
+      <c r="H9" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I9" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
@@ -1295,15 +1130,23 @@
       <c r="D10" s="13"/>
       <c r="E10" s="14"/>
       <c r="F10" s="10">
-        <f>ABS(C10-D10)</f>
+        <f t="shared" si="0"/>
         <v>43.654000000000003</v>
       </c>
       <c r="G10" s="11">
-        <f>ABS(C10-E10)</f>
+        <f t="shared" si="1"/>
         <v>43.654000000000003</v>
       </c>
-    </row>
-    <row r="11">
+      <c r="H10" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I10" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>16</v>
       </c>
@@ -1316,15 +1159,23 @@
       <c r="D11" s="13"/>
       <c r="E11" s="14"/>
       <c r="F11" s="10">
-        <f>ABS(C11-D11)</f>
+        <f t="shared" si="0"/>
         <v>46.249000000000002</v>
       </c>
       <c r="G11" s="11">
-        <f>ABS(C11-E11)</f>
+        <f t="shared" si="1"/>
         <v>46.249000000000002</v>
       </c>
-    </row>
-    <row r="12">
+      <c r="H11" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I11" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>17</v>
       </c>
@@ -1337,15 +1188,23 @@
       <c r="D12" s="13"/>
       <c r="E12" s="14"/>
       <c r="F12" s="10">
-        <f>ABS(C12-D12)</f>
+        <f t="shared" si="0"/>
         <v>48.999000000000002</v>
       </c>
       <c r="G12" s="11">
-        <f>ABS(C12-E12)</f>
+        <f t="shared" si="1"/>
         <v>48.999000000000002</v>
       </c>
-    </row>
-    <row r="13">
+      <c r="H12" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I12" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>18</v>
       </c>
@@ -1358,15 +1217,23 @@
       <c r="D13" s="13"/>
       <c r="E13" s="14"/>
       <c r="F13" s="10">
-        <f>ABS(C13-D13)</f>
+        <f t="shared" si="0"/>
         <v>51.912999999999997</v>
       </c>
       <c r="G13" s="11">
-        <f>ABS(C13-E13)</f>
+        <f t="shared" si="1"/>
         <v>51.912999999999997</v>
       </c>
-    </row>
-    <row r="14">
+      <c r="H13" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I13" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>19</v>
       </c>
@@ -1379,15 +1246,23 @@
       <c r="D14" s="13"/>
       <c r="E14" s="14"/>
       <c r="F14" s="10">
-        <f>ABS(C14-D14)</f>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="G14" s="11">
-        <f>ABS(C14-E14)</f>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="15">
+      <c r="H14" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I14" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>20</v>
       </c>
@@ -1395,20 +1270,28 @@
         <v>34</v>
       </c>
       <c r="C15" s="13">
-        <v>58.270000000000003</v>
+        <v>58.27</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="14"/>
       <c r="F15" s="10">
-        <f>ABS(C15-D15)</f>
-        <v>58.270000000000003</v>
+        <f t="shared" si="0"/>
+        <v>58.27</v>
       </c>
       <c r="G15" s="11">
-        <f>ABS(C15-E15)</f>
-        <v>58.270000000000003</v>
-      </c>
-    </row>
-    <row r="16">
+        <f t="shared" si="1"/>
+        <v>58.27</v>
+      </c>
+      <c r="H15" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I15" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>21</v>
       </c>
@@ -1421,18 +1304,26 @@
       <c r="D16" s="13"/>
       <c r="E16" s="15"/>
       <c r="F16" s="10">
-        <f>ABS(C16-D16)</f>
+        <f t="shared" si="0"/>
         <v>61.734999999999999</v>
       </c>
       <c r="G16" s="11">
-        <f>ABS(C16-E16)</f>
+        <f t="shared" si="1"/>
         <v>61.734999999999999</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I16" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J16" s="21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>23</v>
       </c>
@@ -1447,15 +1338,23 @@
         <v>65</v>
       </c>
       <c r="F17" s="10">
-        <f>ABS(C17-D17)</f>
+        <f t="shared" si="0"/>
         <v>65.406000000000006</v>
       </c>
       <c r="G17" s="11">
-        <f>ABS(C17-E17)</f>
+        <f t="shared" si="1"/>
         <v>0.40600000000000591</v>
       </c>
-    </row>
-    <row r="18">
+      <c r="H17" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I17" s="26">
+        <f t="shared" si="3"/>
+        <v>6.2461538461539368E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>24</v>
       </c>
@@ -1470,15 +1369,23 @@
         <v>70</v>
       </c>
       <c r="F18" s="10">
-        <f>ABS(C18-D18)</f>
+        <f t="shared" si="0"/>
         <v>69.296000000000006</v>
       </c>
       <c r="G18" s="11">
-        <f>ABS(C18-E18)</f>
+        <f t="shared" si="1"/>
         <v>0.70399999999999352</v>
       </c>
-    </row>
-    <row r="19">
+      <c r="H18" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I18" s="26">
+        <f t="shared" si="3"/>
+        <v>1.0057142857142765E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>25</v>
       </c>
@@ -1493,15 +1400,23 @@
         <v>73</v>
       </c>
       <c r="F19" s="10">
-        <f>ABS(C19-D19)</f>
+        <f t="shared" si="0"/>
         <v>73.415999999999997</v>
       </c>
       <c r="G19" s="11">
-        <f>ABS(C19-E19)</f>
+        <f t="shared" si="1"/>
         <v>0.41599999999999682</v>
       </c>
-    </row>
-    <row r="20">
+      <c r="H19" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" s="26">
+        <f t="shared" si="3"/>
+        <v>5.6986301369862579E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>26</v>
       </c>
@@ -1516,15 +1431,23 @@
         <v>79</v>
       </c>
       <c r="F20" s="10">
-        <f>ABS(C20-D20)</f>
+        <f t="shared" si="0"/>
         <v>77.781999999999996</v>
       </c>
       <c r="G20" s="11">
-        <f>ABS(C20-E20)</f>
+        <f t="shared" si="1"/>
         <v>1.2180000000000035</v>
       </c>
-    </row>
-    <row r="21">
+      <c r="H20" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I20" s="26">
+        <f t="shared" si="3"/>
+        <v>1.5417721518987387E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>27</v>
       </c>
@@ -1539,15 +1462,23 @@
         <v>82</v>
       </c>
       <c r="F21" s="10">
-        <f>ABS(C21-D21)</f>
+        <f t="shared" si="0"/>
         <v>82.406999999999996</v>
       </c>
       <c r="G21" s="11">
-        <f>ABS(C21-E21)</f>
+        <f t="shared" si="1"/>
         <v>0.40699999999999648</v>
       </c>
-    </row>
-    <row r="22">
+      <c r="H21" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I21" s="26">
+        <f t="shared" si="3"/>
+        <v>4.9634146341462982E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>28</v>
       </c>
@@ -1562,15 +1493,23 @@
         <v>88</v>
       </c>
       <c r="F22" s="10">
-        <f>ABS(C22-D22)</f>
+        <f t="shared" si="0"/>
         <v>87.307000000000002</v>
       </c>
       <c r="G22" s="11">
-        <f>ABS(C22-E22)</f>
+        <f t="shared" si="1"/>
         <v>0.69299999999999784</v>
       </c>
-    </row>
-    <row r="23">
+      <c r="H22" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I22" s="26">
+        <f t="shared" si="3"/>
+        <v>7.8749999999999758E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>29</v>
       </c>
@@ -1585,15 +1524,23 @@
         <v>94</v>
       </c>
       <c r="F23" s="10">
-        <f>ABS(C23-D23)</f>
+        <f t="shared" si="0"/>
         <v>92.498999999999995</v>
       </c>
       <c r="G23" s="11">
-        <f>ABS(C23-E23)</f>
+        <f t="shared" si="1"/>
         <v>1.5010000000000048</v>
       </c>
-    </row>
-    <row r="24">
+      <c r="H23" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I23" s="26">
+        <f t="shared" si="3"/>
+        <v>1.5968085106383031E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>30</v>
       </c>
@@ -1608,15 +1555,23 @@
         <v>97</v>
       </c>
       <c r="F24" s="10">
-        <f>ABS(C24-D24)</f>
+        <f t="shared" si="0"/>
         <v>97.998999999999995</v>
       </c>
       <c r="G24" s="11">
-        <f>ABS(C24-E24)</f>
+        <f t="shared" si="1"/>
         <v>0.99899999999999523</v>
       </c>
-    </row>
-    <row r="25">
+      <c r="H24" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I24" s="26">
+        <f t="shared" si="3"/>
+        <v>1.0298969072164899E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>31</v>
       </c>
@@ -1631,15 +1586,23 @@
         <v>103</v>
       </c>
       <c r="F25" s="10">
-        <f>ABS(C25-D25)</f>
+        <f t="shared" si="0"/>
         <v>103.83</v>
       </c>
       <c r="G25" s="11">
-        <f>ABS(C25-E25)</f>
+        <f t="shared" si="1"/>
         <v>0.82999999999999829</v>
       </c>
-    </row>
-    <row r="26">
+      <c r="H25" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I25" s="26">
+        <f t="shared" si="3"/>
+        <v>8.0582524271844494E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>32</v>
       </c>
@@ -1654,15 +1617,23 @@
         <v>111</v>
       </c>
       <c r="F26" s="10">
-        <f>ABS(C26-D26)</f>
+        <f t="shared" si="0"/>
         <v>110</v>
       </c>
       <c r="G26" s="11">
-        <f>ABS(C26-E26)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="27">
+      <c r="H26" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I26" s="26">
+        <f t="shared" si="3"/>
+        <v>9.0090090090090089E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>33</v>
       </c>
@@ -1670,22 +1641,30 @@
         <v>46</v>
       </c>
       <c r="C27" s="13">
-        <v>116.54000000000001</v>
+        <v>116.54</v>
       </c>
       <c r="D27" s="13"/>
       <c r="E27" s="14">
         <v>117</v>
       </c>
       <c r="F27" s="10">
-        <f>ABS(C27-D27)</f>
-        <v>116.54000000000001</v>
+        <f t="shared" si="0"/>
+        <v>116.54</v>
       </c>
       <c r="G27" s="11">
-        <f>ABS(C27-E27)</f>
+        <f t="shared" si="1"/>
         <v>0.45999999999999375</v>
       </c>
-    </row>
-    <row r="28">
+      <c r="H27" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I27" s="26">
+        <f t="shared" si="3"/>
+        <v>3.9316239316238783E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>34</v>
       </c>
@@ -1700,15 +1679,23 @@
         <v>123</v>
       </c>
       <c r="F28" s="10">
-        <f>ABS(C28-D28)</f>
+        <f t="shared" si="0"/>
         <v>123.47</v>
       </c>
       <c r="G28" s="11">
-        <f>ABS(C28-E28)</f>
+        <f t="shared" si="1"/>
         <v>0.46999999999999886</v>
       </c>
-    </row>
-    <row r="29">
+      <c r="H28" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I28" s="26">
+        <f t="shared" si="3"/>
+        <v>3.8211382113821045E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>35</v>
       </c>
@@ -1723,15 +1710,23 @@
         <v>132</v>
       </c>
       <c r="F29" s="10">
-        <f>ABS(C29-D29)</f>
+        <f t="shared" si="0"/>
         <v>130.81</v>
       </c>
       <c r="G29" s="11">
-        <f>ABS(C29-E29)</f>
+        <f t="shared" si="1"/>
         <v>1.1899999999999977</v>
       </c>
-    </row>
-    <row r="30">
+      <c r="H29" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I29" s="26">
+        <f t="shared" si="3"/>
+        <v>9.0151515151514986E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>36</v>
       </c>
@@ -1746,15 +1741,23 @@
         <v>138</v>
       </c>
       <c r="F30" s="10">
-        <f>ABS(C30-D30)</f>
+        <f t="shared" si="0"/>
         <v>138.59</v>
       </c>
       <c r="G30" s="11">
-        <f>ABS(C30-E30)</f>
+        <f t="shared" si="1"/>
         <v>0.59000000000000341</v>
       </c>
-    </row>
-    <row r="31">
+      <c r="H30" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I30" s="26">
+        <f t="shared" si="3"/>
+        <v>4.2753623188406045E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>37</v>
       </c>
@@ -1769,15 +1772,23 @@
         <v>146</v>
       </c>
       <c r="F31" s="10">
-        <f>ABS(C31-D31)</f>
+        <f t="shared" si="0"/>
         <v>146.83000000000001</v>
       </c>
       <c r="G31" s="11">
-        <f>ABS(C31-E31)</f>
+        <f t="shared" si="1"/>
         <v>0.83000000000001251</v>
       </c>
-    </row>
-    <row r="32">
+      <c r="H31" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I31" s="26">
+        <f t="shared" si="3"/>
+        <v>5.6849315068494008E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>38</v>
       </c>
@@ -1794,15 +1805,23 @@
         <v>155</v>
       </c>
       <c r="F32" s="10">
-        <f>ABS(C32-D32)</f>
-        <v>4.0999999999996817e-002</v>
+        <f t="shared" si="0"/>
+        <v>4.0999999999996817E-2</v>
       </c>
       <c r="G32" s="11">
-        <f>ABS(C32-E32)</f>
+        <f t="shared" si="1"/>
         <v>0.56000000000000227</v>
       </c>
-    </row>
-    <row r="33">
+      <c r="H32" s="23">
+        <f t="shared" si="2"/>
+        <v>2.6349445054978321E-4</v>
+      </c>
+      <c r="I32" s="26">
+        <f t="shared" si="3"/>
+        <v>3.6129032258064662E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>39</v>
       </c>
@@ -1819,15 +1838,23 @@
         <v>164</v>
       </c>
       <c r="F33" s="10">
-        <f>ABS(C33-D33)</f>
-        <v>2.5000000000005684e-002</v>
+        <f t="shared" si="0"/>
+        <v>2.5000000000005684E-2</v>
       </c>
       <c r="G33" s="11">
-        <f>ABS(C33-E33)</f>
+        <f t="shared" si="1"/>
         <v>0.81000000000000227</v>
       </c>
-    </row>
-    <row r="34">
+      <c r="H33" s="23">
+        <f t="shared" si="2"/>
+        <v>1.5166681833351947E-4</v>
+      </c>
+      <c r="I33" s="26">
+        <f t="shared" si="3"/>
+        <v>4.9390243902439164E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>40</v>
       </c>
@@ -1835,7 +1862,7 @@
         <v>53</v>
       </c>
       <c r="C34" s="13">
-        <v>174.61000000000001</v>
+        <v>174.61</v>
       </c>
       <c r="D34" s="13">
         <v>174.476</v>
@@ -1844,15 +1871,23 @@
         <v>176</v>
       </c>
       <c r="F34" s="10">
-        <f>ABS(C34-D34)</f>
+        <f t="shared" ref="F34:F65" si="4">ABS(C34-D34)</f>
         <v>0.13400000000001455</v>
       </c>
       <c r="G34" s="11">
-        <f>ABS(C34-E34)</f>
+        <f t="shared" ref="G34:G65" si="5">ABS(C34-E34)</f>
         <v>1.3899999999999864</v>
       </c>
-    </row>
-    <row r="35">
+      <c r="H34" s="23">
+        <f t="shared" si="2"/>
+        <v>7.6801393887992932E-4</v>
+      </c>
+      <c r="I34" s="26">
+        <f t="shared" si="3"/>
+        <v>7.8977272727271952E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>41</v>
       </c>
@@ -1869,15 +1904,23 @@
         <v>185</v>
       </c>
       <c r="F35" s="10">
-        <f>ABS(C35-D35)</f>
-        <v>1.099999999999568e-002</v>
+        <f t="shared" si="4"/>
+        <v>1.099999999999568E-2</v>
       </c>
       <c r="G35" s="11">
-        <f>ABS(C35-E35)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="36">
+      <c r="H35" s="23">
+        <f t="shared" si="2"/>
+        <v>5.9462995096982416E-5</v>
+      </c>
+      <c r="I35" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>42</v>
       </c>
@@ -1894,15 +1937,23 @@
         <v>196</v>
       </c>
       <c r="F36" s="10">
-        <f>ABS(C36-D36)</f>
-        <v>7.8000000000002956e-002</v>
+        <f t="shared" si="4"/>
+        <v>7.8000000000002956E-2</v>
       </c>
       <c r="G36" s="11">
-        <f>ABS(C36-E36)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="37">
+      <c r="H36" s="23">
+        <f t="shared" si="2"/>
+        <v>3.9780087516194044E-4</v>
+      </c>
+      <c r="I36" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>43</v>
       </c>
@@ -1910,7 +1961,7 @@
         <v>56</v>
       </c>
       <c r="C37" s="13">
-        <v>207.65000000000001</v>
+        <v>207.65</v>
       </c>
       <c r="D37" s="13">
         <v>207.46799999999999</v>
@@ -1919,15 +1970,23 @@
         <v>208</v>
       </c>
       <c r="F37" s="10">
-        <f>ABS(C37-D37)</f>
+        <f t="shared" si="4"/>
         <v>0.18200000000001637</v>
       </c>
       <c r="G37" s="11">
-        <f>ABS(C37-E37)</f>
+        <f t="shared" si="5"/>
         <v>0.34999999999999432</v>
       </c>
-    </row>
-    <row r="38">
+      <c r="H37" s="23">
+        <f t="shared" si="2"/>
+        <v>8.7724371951344968E-4</v>
+      </c>
+      <c r="I37" s="26">
+        <f t="shared" si="3"/>
+        <v>1.6826923076922805E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>44</v>
       </c>
@@ -1944,15 +2003,23 @@
         <v>220</v>
       </c>
       <c r="F38" s="10">
-        <f>ABS(C38-D38)</f>
-        <v>2.199999999999136e-002</v>
+        <f t="shared" si="4"/>
+        <v>2.199999999999136E-2</v>
       </c>
       <c r="G38" s="11">
-        <f>ABS(C38-E38)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="39">
+      <c r="H38" s="23">
+        <f t="shared" si="2"/>
+        <v>9.999000099986074E-5</v>
+      </c>
+      <c r="I38" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>45</v>
       </c>
@@ -1960,7 +2027,7 @@
         <v>58</v>
       </c>
       <c r="C39" s="13">
-        <v>233.08000000000001</v>
+        <v>233.08</v>
       </c>
       <c r="D39" s="13">
         <v>233.16</v>
@@ -1969,15 +2036,23 @@
         <v>234</v>
       </c>
       <c r="F39" s="10">
-        <f>ABS(C39-D39)</f>
-        <v>7.9999999999984084e-002</v>
+        <f t="shared" si="4"/>
+        <v>7.9999999999984084E-2</v>
       </c>
       <c r="G39" s="11">
-        <f>ABS(C39-E39)</f>
+        <f t="shared" si="5"/>
         <v>0.91999999999998749</v>
       </c>
-    </row>
-    <row r="40">
+      <c r="H39" s="23">
+        <f t="shared" si="2"/>
+        <v>3.4311202607644571E-4</v>
+      </c>
+      <c r="I39" s="26">
+        <f t="shared" si="3"/>
+        <v>3.9316239316238783E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>46</v>
       </c>
@@ -1994,15 +2069,23 @@
         <v>246</v>
       </c>
       <c r="F40" s="10">
-        <f>ABS(C40-D40)</f>
-        <v>9.4999999999998863e-002</v>
+        <f t="shared" si="4"/>
+        <v>9.4999999999998863E-2</v>
       </c>
       <c r="G40" s="11">
-        <f>ABS(C40-E40)</f>
+        <f t="shared" si="5"/>
         <v>0.93999999999999773</v>
       </c>
-    </row>
-    <row r="41">
+      <c r="H40" s="23">
+        <f t="shared" si="2"/>
+        <v>3.8456089218126527E-4</v>
+      </c>
+      <c r="I40" s="26">
+        <f t="shared" si="3"/>
+        <v>3.8211382113821045E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>47</v>
       </c>
@@ -2019,15 +2102,23 @@
         <v>261</v>
       </c>
       <c r="F41" s="10">
-        <f>ABS(C41-D41)</f>
+        <f t="shared" si="4"/>
         <v>0.15800000000001546</v>
       </c>
       <c r="G41" s="11">
-        <f>ABS(C41-E41)</f>
+        <f t="shared" si="5"/>
         <v>0.62999999999999545</v>
       </c>
-    </row>
-    <row r="42">
+      <c r="H41" s="23">
+        <f t="shared" si="2"/>
+        <v>6.035417971794561E-4</v>
+      </c>
+      <c r="I41" s="26">
+        <f t="shared" si="3"/>
+        <v>2.4137931034482587E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>48</v>
       </c>
@@ -2035,7 +2126,7 @@
         <v>61</v>
       </c>
       <c r="C42" s="13">
-        <v>277.18000000000001</v>
+        <v>277.18</v>
       </c>
       <c r="D42" s="13">
         <v>277.21699999999998</v>
@@ -2044,15 +2135,23 @@
         <v>278</v>
       </c>
       <c r="F42" s="10">
-        <f>ABS(C42-D42)</f>
-        <v>3.6999999999977717e-002</v>
+        <f t="shared" si="4"/>
+        <v>3.6999999999977717E-2</v>
       </c>
       <c r="G42" s="11">
-        <f>ABS(C42-E42)</f>
+        <f t="shared" si="5"/>
         <v>0.81999999999999318</v>
       </c>
-    </row>
-    <row r="43">
+      <c r="H42" s="23">
+        <f t="shared" si="2"/>
+        <v>1.3346944812178807E-4</v>
+      </c>
+      <c r="I42" s="26">
+        <f t="shared" si="3"/>
+        <v>2.9496402877697597E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>49</v>
       </c>
@@ -2060,7 +2159,7 @@
         <v>62</v>
       </c>
       <c r="C43" s="13">
-        <v>293.67000000000002</v>
+        <v>293.67</v>
       </c>
       <c r="D43" s="13">
         <v>293.82900000000001</v>
@@ -2069,15 +2168,23 @@
         <v>293</v>
       </c>
       <c r="F43" s="10">
-        <f>ABS(C43-D43)</f>
+        <f t="shared" si="4"/>
         <v>0.15899999999999181</v>
       </c>
       <c r="G43" s="11">
-        <f>ABS(C43-E43)</f>
+        <f t="shared" si="5"/>
         <v>0.67000000000001592</v>
       </c>
-    </row>
-    <row r="44">
+      <c r="H43" s="23">
+        <f t="shared" si="2"/>
+        <v>5.4113106602817222E-4</v>
+      </c>
+      <c r="I43" s="26">
+        <f t="shared" si="3"/>
+        <v>2.286689419795276E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>50</v>
       </c>
@@ -2094,15 +2201,23 @@
         <v>311</v>
       </c>
       <c r="F44" s="10">
-        <f>ABS(C44-D44)</f>
-        <v>7.2999999999979082e-002</v>
+        <f t="shared" si="4"/>
+        <v>7.2999999999979082E-2</v>
       </c>
       <c r="G44" s="11">
-        <f>ABS(C44-E44)</f>
+        <f t="shared" si="5"/>
         <v>0.12999999999999545</v>
       </c>
-    </row>
-    <row r="45">
+      <c r="H44" s="23">
+        <f t="shared" si="2"/>
+        <v>2.3457357416213561E-4</v>
+      </c>
+      <c r="I44" s="26">
+        <f t="shared" si="3"/>
+        <v>4.1800643086815258E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>51</v>
       </c>
@@ -2110,7 +2225,7 @@
         <v>64</v>
       </c>
       <c r="C45" s="13">
-        <v>329.23000000000002</v>
+        <v>329.23</v>
       </c>
       <c r="D45" s="13">
         <v>329.61399999999998</v>
@@ -2119,15 +2234,23 @@
         <v>331</v>
       </c>
       <c r="F45" s="10">
-        <f>ABS(C45-D45)</f>
+        <f t="shared" si="4"/>
         <v>0.38399999999995771</v>
       </c>
       <c r="G45" s="11">
-        <f>ABS(C45-E45)</f>
+        <f t="shared" si="5"/>
         <v>1.7699999999999818</v>
       </c>
-    </row>
-    <row r="46">
+      <c r="H45" s="23">
+        <f t="shared" si="2"/>
+        <v>1.1649990595058394E-3</v>
+      </c>
+      <c r="I45" s="26">
+        <f t="shared" si="3"/>
+        <v>5.3474320241691294E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>52</v>
       </c>
@@ -2135,7 +2258,7 @@
         <v>65</v>
       </c>
       <c r="C46" s="13">
-        <v>349.23000000000002</v>
+        <v>349.23</v>
       </c>
       <c r="D46" s="13">
         <v>349.30099999999999</v>
@@ -2144,15 +2267,23 @@
         <v>349</v>
       </c>
       <c r="F46" s="10">
-        <f>ABS(C46-D46)</f>
-        <v>7.0999999999969532e-002</v>
+        <f t="shared" si="4"/>
+        <v>7.0999999999969532E-2</v>
       </c>
       <c r="G46" s="11">
-        <f>ABS(C46-E46)</f>
+        <f t="shared" si="5"/>
         <v>0.23000000000001819</v>
       </c>
-    </row>
-    <row r="47">
+      <c r="H46" s="23">
+        <f t="shared" si="2"/>
+        <v>2.0326308828193888E-4</v>
+      </c>
+      <c r="I46" s="26">
+        <f t="shared" si="3"/>
+        <v>6.5902578796566812E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>53</v>
       </c>
@@ -2160,7 +2291,7 @@
         <v>66</v>
       </c>
       <c r="C47" s="13">
-        <v>369.99000000000001</v>
+        <v>369.99</v>
       </c>
       <c r="D47" s="1">
         <v>369.822</v>
@@ -2169,15 +2300,23 @@
         <v>369</v>
       </c>
       <c r="F47" s="10">
-        <f>ABS(C47-D47)</f>
+        <f t="shared" si="4"/>
         <v>0.16800000000000637</v>
       </c>
       <c r="G47" s="11">
-        <f>ABS(C47-E47)</f>
+        <f t="shared" si="5"/>
         <v>0.99000000000000909</v>
       </c>
-    </row>
-    <row r="48">
+      <c r="H47" s="23">
+        <f t="shared" si="2"/>
+        <v>4.5427259600566315E-4</v>
+      </c>
+      <c r="I47" s="26">
+        <f t="shared" si="3"/>
+        <v>2.6829268292683172E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>54</v>
       </c>
@@ -2194,15 +2333,23 @@
         <v>393</v>
       </c>
       <c r="F48" s="10">
-        <f>ABS(C48-D48)</f>
+        <f t="shared" si="4"/>
         <v>0.15600000000000591</v>
       </c>
       <c r="G48" s="11">
-        <f>ABS(C48-E48)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="49">
+      <c r="H48" s="23">
+        <f t="shared" si="2"/>
+        <v>3.9780087516194044E-4</v>
+      </c>
+      <c r="I48" s="26">
+        <f t="shared" si="3"/>
+        <v>2.5445292620865142E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>55</v>
       </c>
@@ -2210,7 +2357,7 @@
         <v>68</v>
       </c>
       <c r="C49" s="13">
-        <v>415.30000000000001</v>
+        <v>415.3</v>
       </c>
       <c r="D49" s="13">
         <v>414.93700000000001</v>
@@ -2219,15 +2366,23 @@
         <v>416</v>
       </c>
       <c r="F49" s="10">
-        <f>ABS(C49-D49)</f>
+        <f t="shared" si="4"/>
         <v>0.36299999999999955</v>
       </c>
       <c r="G49" s="11">
-        <f>ABS(C49-E49)</f>
+        <f t="shared" si="5"/>
         <v>0.69999999999998863</v>
       </c>
-    </row>
-    <row r="50">
+      <c r="H49" s="23">
+        <f t="shared" si="2"/>
+        <v>8.7483160094182859E-4</v>
+      </c>
+      <c r="I49" s="26">
+        <f t="shared" si="3"/>
+        <v>1.6826923076922805E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>56</v>
       </c>
@@ -2244,15 +2399,23 @@
         <v>439</v>
       </c>
       <c r="F50" s="10">
-        <f>ABS(C50-D50)</f>
-        <v>4.199999999997317e-002</v>
+        <f t="shared" si="4"/>
+        <v>4.199999999997317E-2</v>
       </c>
       <c r="G50" s="11">
-        <f>ABS(C50-E50)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="51">
+      <c r="H50" s="23">
+        <f t="shared" si="2"/>
+        <v>9.546365789455622E-5</v>
+      </c>
+      <c r="I50" s="26">
+        <f t="shared" si="3"/>
+        <v>2.2779043280182231E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>57</v>
       </c>
@@ -2260,20 +2423,28 @@
         <v>70</v>
       </c>
       <c r="C51" s="13">
-        <v>466.16000000000003</v>
+        <v>466.16</v>
       </c>
       <c r="D51" s="13"/>
       <c r="E51" s="14"/>
       <c r="F51" s="10">
-        <f>ABS(C51-D51)</f>
-        <v>466.16000000000003</v>
+        <f t="shared" si="4"/>
+        <v>466.16</v>
       </c>
       <c r="G51" s="11">
-        <f>ABS(C51-E51)</f>
-        <v>466.16000000000003</v>
-      </c>
-    </row>
-    <row r="52">
+        <f t="shared" si="5"/>
+        <v>466.16</v>
+      </c>
+      <c r="H51" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I51" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>58</v>
       </c>
@@ -2286,15 +2457,23 @@
       <c r="D52" s="13"/>
       <c r="E52" s="14"/>
       <c r="F52" s="10">
-        <f>ABS(C52-D52)</f>
+        <f t="shared" si="4"/>
         <v>493.88</v>
       </c>
       <c r="G52" s="11">
-        <f>ABS(C52-E52)</f>
+        <f t="shared" si="5"/>
         <v>493.88</v>
       </c>
-    </row>
-    <row r="53">
+      <c r="H52" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I52" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>59</v>
       </c>
@@ -2307,15 +2486,23 @@
       <c r="D53" s="13"/>
       <c r="E53" s="14"/>
       <c r="F53" s="10">
-        <f>ABS(C53-D53)</f>
+        <f t="shared" si="4"/>
         <v>523.25</v>
       </c>
       <c r="G53" s="11">
-        <f>ABS(C53-E53)</f>
+        <f t="shared" si="5"/>
         <v>523.25</v>
       </c>
-    </row>
-    <row r="54">
+      <c r="H53" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I53" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>60</v>
       </c>
@@ -2328,15 +2515,23 @@
       <c r="D54" s="13"/>
       <c r="E54" s="14"/>
       <c r="F54" s="10">
-        <f>ABS(C54-D54)</f>
+        <f t="shared" si="4"/>
         <v>554.37</v>
       </c>
       <c r="G54" s="11">
-        <f>ABS(C54-E54)</f>
+        <f t="shared" si="5"/>
         <v>554.37</v>
       </c>
-    </row>
-    <row r="55">
+      <c r="H54" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I54" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>61</v>
       </c>
@@ -2349,15 +2544,23 @@
       <c r="D55" s="13"/>
       <c r="E55" s="14"/>
       <c r="F55" s="10">
-        <f>ABS(C55-D55)</f>
+        <f t="shared" si="4"/>
         <v>587.33000000000004</v>
       </c>
       <c r="G55" s="11">
-        <f>ABS(C55-E55)</f>
+        <f t="shared" si="5"/>
         <v>587.33000000000004</v>
       </c>
-    </row>
-    <row r="56">
+      <c r="H55" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I55" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>62</v>
       </c>
@@ -2370,15 +2573,23 @@
       <c r="D56" s="13"/>
       <c r="E56" s="14"/>
       <c r="F56" s="10">
-        <f>ABS(C56-D56)</f>
+        <f t="shared" si="4"/>
         <v>622.25</v>
       </c>
       <c r="G56" s="11">
-        <f>ABS(C56-E56)</f>
+        <f t="shared" si="5"/>
         <v>622.25</v>
       </c>
-    </row>
-    <row r="57">
+      <c r="H56" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I56" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>63</v>
       </c>
@@ -2386,20 +2597,28 @@
         <v>76</v>
       </c>
       <c r="C57" s="13">
-        <v>659.25999999999999</v>
+        <v>659.26</v>
       </c>
       <c r="D57" s="13"/>
       <c r="E57" s="14"/>
       <c r="F57" s="10">
-        <f>ABS(C57-D57)</f>
-        <v>659.25999999999999</v>
+        <f t="shared" si="4"/>
+        <v>659.26</v>
       </c>
       <c r="G57" s="11">
-        <f>ABS(C57-E57)</f>
-        <v>659.25999999999999</v>
-      </c>
-    </row>
-    <row r="58">
+        <f t="shared" si="5"/>
+        <v>659.26</v>
+      </c>
+      <c r="H57" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I57" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>64</v>
       </c>
@@ -2407,20 +2626,28 @@
         <v>77</v>
       </c>
       <c r="C58" s="13">
-        <v>698.46000000000004</v>
+        <v>698.46</v>
       </c>
       <c r="D58" s="13"/>
       <c r="E58" s="14"/>
       <c r="F58" s="10">
-        <f>ABS(C58-D58)</f>
-        <v>698.46000000000004</v>
+        <f t="shared" si="4"/>
+        <v>698.46</v>
       </c>
       <c r="G58" s="11">
-        <f>ABS(C58-E58)</f>
-        <v>698.46000000000004</v>
-      </c>
-    </row>
-    <row r="59">
+        <f t="shared" si="5"/>
+        <v>698.46</v>
+      </c>
+      <c r="H58" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I58" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>65</v>
       </c>
@@ -2428,20 +2655,28 @@
         <v>78</v>
       </c>
       <c r="C59" s="13">
-        <v>739.99000000000001</v>
+        <v>739.99</v>
       </c>
       <c r="D59" s="13"/>
       <c r="E59" s="14"/>
       <c r="F59" s="10">
-        <f>ABS(C59-D59)</f>
-        <v>739.99000000000001</v>
+        <f t="shared" si="4"/>
+        <v>739.99</v>
       </c>
       <c r="G59" s="11">
-        <f>ABS(C59-E59)</f>
-        <v>739.99000000000001</v>
-      </c>
-    </row>
-    <row r="60">
+        <f t="shared" si="5"/>
+        <v>739.99</v>
+      </c>
+      <c r="H59" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I59" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>66</v>
       </c>
@@ -2449,20 +2684,28 @@
         <v>79</v>
       </c>
       <c r="C60" s="13">
-        <v>783.99000000000001</v>
+        <v>783.99</v>
       </c>
       <c r="D60" s="13"/>
       <c r="E60" s="14"/>
       <c r="F60" s="10">
-        <f>ABS(C60-D60)</f>
-        <v>783.99000000000001</v>
+        <f t="shared" si="4"/>
+        <v>783.99</v>
       </c>
       <c r="G60" s="11">
-        <f>ABS(C60-E60)</f>
-        <v>783.99000000000001</v>
-      </c>
-    </row>
-    <row r="61">
+        <f t="shared" si="5"/>
+        <v>783.99</v>
+      </c>
+      <c r="H60" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I60" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>67</v>
       </c>
@@ -2470,20 +2713,28 @@
         <v>80</v>
       </c>
       <c r="C61" s="13">
-        <v>830.61000000000001</v>
+        <v>830.61</v>
       </c>
       <c r="D61" s="13"/>
       <c r="E61" s="14"/>
       <c r="F61" s="10">
-        <f>ABS(C61-D61)</f>
-        <v>830.61000000000001</v>
+        <f t="shared" si="4"/>
+        <v>830.61</v>
       </c>
       <c r="G61" s="11">
-        <f>ABS(C61-E61)</f>
-        <v>830.61000000000001</v>
-      </c>
-    </row>
-    <row r="62">
+        <f t="shared" si="5"/>
+        <v>830.61</v>
+      </c>
+      <c r="H61" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I61" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
         <v>68</v>
       </c>
@@ -2496,15 +2747,23 @@
       <c r="D62" s="13"/>
       <c r="E62" s="14"/>
       <c r="F62" s="10">
-        <f>ABS(C62-D62)</f>
+        <f t="shared" si="4"/>
         <v>880</v>
       </c>
       <c r="G62" s="11">
-        <f>ABS(C62-E62)</f>
+        <f t="shared" si="5"/>
         <v>880</v>
       </c>
-    </row>
-    <row r="63">
+      <c r="H62" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I62" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
         <v>69</v>
       </c>
@@ -2512,20 +2771,28 @@
         <v>82</v>
       </c>
       <c r="C63" s="13">
-        <v>923.33000000000004</v>
+        <v>923.33</v>
       </c>
       <c r="D63" s="13"/>
       <c r="E63" s="14"/>
       <c r="F63" s="10">
-        <f>ABS(C63-D63)</f>
-        <v>923.33000000000004</v>
+        <f t="shared" si="4"/>
+        <v>923.33</v>
       </c>
       <c r="G63" s="11">
-        <f>ABS(C63-E63)</f>
-        <v>923.33000000000004</v>
-      </c>
-    </row>
-    <row r="64">
+        <f t="shared" si="5"/>
+        <v>923.33</v>
+      </c>
+      <c r="H63" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I63" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
         <v>70</v>
       </c>
@@ -2533,20 +2800,28 @@
         <v>83</v>
       </c>
       <c r="C64" s="13">
-        <v>987.76999999999998</v>
+        <v>987.77</v>
       </c>
       <c r="D64" s="13"/>
       <c r="E64" s="14"/>
       <c r="F64" s="10">
-        <f>ABS(C64-D64)</f>
-        <v>987.76999999999998</v>
+        <f t="shared" si="4"/>
+        <v>987.77</v>
       </c>
       <c r="G64" s="11">
-        <f>ABS(C64-E64)</f>
-        <v>987.76999999999998</v>
-      </c>
-    </row>
-    <row r="65">
+        <f t="shared" si="5"/>
+        <v>987.77</v>
+      </c>
+      <c r="H64" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I64" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
         <v>71</v>
       </c>
@@ -2559,15 +2834,23 @@
       <c r="D65" s="13"/>
       <c r="E65" s="14"/>
       <c r="F65" s="10">
-        <f>ABS(C65-D65)</f>
+        <f t="shared" si="4"/>
         <v>1046.5</v>
       </c>
       <c r="G65" s="11">
-        <f>ABS(C65-E65)</f>
+        <f t="shared" si="5"/>
         <v>1046.5</v>
       </c>
-    </row>
-    <row r="66">
+      <c r="H65" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I65" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
         <v>72</v>
       </c>
@@ -2580,15 +2863,23 @@
       <c r="D66" s="13"/>
       <c r="E66" s="14"/>
       <c r="F66" s="10">
-        <f>ABS(C66-D66)</f>
+        <f t="shared" ref="F66:F89" si="6">ABS(C66-D66)</f>
         <v>1108.7</v>
       </c>
       <c r="G66" s="11">
-        <f>ABS(C66-E66)</f>
+        <f t="shared" ref="G66:G89" si="7">ABS(C66-E66)</f>
         <v>1108.7</v>
       </c>
-    </row>
-    <row r="67">
+      <c r="H66" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I66" s="26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
         <v>73</v>
       </c>
@@ -2601,15 +2892,23 @@
       <c r="D67" s="13"/>
       <c r="E67" s="14"/>
       <c r="F67" s="10">
-        <f>ABS(C67-D67)</f>
+        <f t="shared" si="6"/>
         <v>1174.7</v>
       </c>
       <c r="G67" s="11">
-        <f>ABS(C67-E67)</f>
+        <f t="shared" si="7"/>
         <v>1174.7</v>
       </c>
-    </row>
-    <row r="68">
+      <c r="H67" s="23" t="e">
+        <f t="shared" ref="H67:H89" si="8">F67/D67</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I67" s="26" t="e">
+        <f t="shared" ref="I67:I89" si="9">G67/E67</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
         <v>74</v>
       </c>
@@ -2622,15 +2921,23 @@
       <c r="D68" s="13"/>
       <c r="E68" s="14"/>
       <c r="F68" s="10">
-        <f>ABS(C68-D68)</f>
+        <f t="shared" si="6"/>
         <v>1244.5</v>
       </c>
       <c r="G68" s="11">
-        <f>ABS(C68-E68)</f>
+        <f t="shared" si="7"/>
         <v>1244.5</v>
       </c>
-    </row>
-    <row r="69">
+      <c r="H68" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I68" s="26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
         <v>75</v>
       </c>
@@ -2643,15 +2950,23 @@
       <c r="D69" s="13"/>
       <c r="E69" s="14"/>
       <c r="F69" s="10">
-        <f>ABS(C69-D69)</f>
+        <f t="shared" si="6"/>
         <v>1318.5</v>
       </c>
       <c r="G69" s="11">
-        <f>ABS(C69-E69)</f>
+        <f t="shared" si="7"/>
         <v>1318.5</v>
       </c>
-    </row>
-    <row r="70">
+      <c r="H69" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I69" s="26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
         <v>76</v>
       </c>
@@ -2659,20 +2974,28 @@
         <v>89</v>
       </c>
       <c r="C70" s="13">
-        <v>1396.9000000000001</v>
+        <v>1396.9</v>
       </c>
       <c r="D70" s="13"/>
       <c r="E70" s="14"/>
       <c r="F70" s="10">
-        <f>ABS(C70-D70)</f>
-        <v>1396.9000000000001</v>
+        <f t="shared" si="6"/>
+        <v>1396.9</v>
       </c>
       <c r="G70" s="11">
-        <f>ABS(C70-E70)</f>
-        <v>1396.9000000000001</v>
-      </c>
-    </row>
-    <row r="71">
+        <f t="shared" si="7"/>
+        <v>1396.9</v>
+      </c>
+      <c r="H70" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I70" s="26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
         <v>77</v>
       </c>
@@ -2685,15 +3008,23 @@
       <c r="D71" s="13"/>
       <c r="E71" s="14"/>
       <c r="F71" s="10">
-        <f>ABS(C71-D71)</f>
+        <f t="shared" si="6"/>
         <v>1480</v>
       </c>
       <c r="G71" s="11">
-        <f>ABS(C71-E71)</f>
+        <f t="shared" si="7"/>
         <v>1480</v>
       </c>
-    </row>
-    <row r="72">
+      <c r="H71" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I71" s="26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
         <v>78</v>
       </c>
@@ -2706,15 +3037,23 @@
       <c r="D72" s="13"/>
       <c r="E72" s="14"/>
       <c r="F72" s="10">
-        <f>ABS(C72-D72)</f>
+        <f t="shared" si="6"/>
         <v>1568</v>
       </c>
       <c r="G72" s="11">
-        <f>ABS(C72-E72)</f>
+        <f t="shared" si="7"/>
         <v>1568</v>
       </c>
-    </row>
-    <row r="73">
+      <c r="H72" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I72" s="26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
         <v>79</v>
       </c>
@@ -2727,15 +3066,23 @@
       <c r="D73" s="13"/>
       <c r="E73" s="14"/>
       <c r="F73" s="10">
-        <f>ABS(C73-D73)</f>
+        <f t="shared" si="6"/>
         <v>1661.2</v>
       </c>
       <c r="G73" s="11">
-        <f>ABS(C73-E73)</f>
+        <f t="shared" si="7"/>
         <v>1661.2</v>
       </c>
-    </row>
-    <row r="74">
+      <c r="H73" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I73" s="26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
         <v>80</v>
       </c>
@@ -2750,15 +3097,23 @@
         <v>1758</v>
       </c>
       <c r="F74" s="10">
-        <f>ABS(C74-D74)</f>
+        <f t="shared" si="6"/>
         <v>1760</v>
       </c>
       <c r="G74" s="11">
-        <f>ABS(C74-E74)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="75">
+      <c r="H74" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I74" s="26">
+        <f t="shared" si="9"/>
+        <v>1.1376564277588168E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
         <v>81</v>
       </c>
@@ -2771,15 +3126,23 @@
       <c r="D75" s="13"/>
       <c r="E75" s="14"/>
       <c r="F75" s="10">
-        <f>ABS(C75-D75)</f>
+        <f t="shared" si="6"/>
         <v>1864.7</v>
       </c>
       <c r="G75" s="11">
-        <f>ABS(C75-E75)</f>
+        <f t="shared" si="7"/>
         <v>1864.7</v>
       </c>
-    </row>
-    <row r="76">
+      <c r="H75" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I75" s="26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
         <v>82</v>
       </c>
@@ -2792,15 +3155,23 @@
       <c r="D76" s="13"/>
       <c r="E76" s="14"/>
       <c r="F76" s="10">
-        <f>ABS(C76-D76)</f>
+        <f t="shared" si="6"/>
         <v>1975.5</v>
       </c>
       <c r="G76" s="11">
-        <f>ABS(C76-E76)</f>
+        <f t="shared" si="7"/>
         <v>1975.5</v>
       </c>
-    </row>
-    <row r="77">
+      <c r="H76" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I76" s="26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
         <v>83</v>
       </c>
@@ -2813,15 +3184,23 @@
       <c r="D77" s="13"/>
       <c r="E77" s="14"/>
       <c r="F77" s="10">
-        <f>ABS(C77-D77)</f>
+        <f t="shared" si="6"/>
         <v>2093</v>
       </c>
       <c r="G77" s="11">
-        <f>ABS(C77-E77)</f>
+        <f t="shared" si="7"/>
         <v>2093</v>
       </c>
-    </row>
-    <row r="78">
+      <c r="H77" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I77" s="26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
         <v>84</v>
       </c>
@@ -2834,15 +3213,23 @@
       <c r="D78" s="13"/>
       <c r="E78" s="14"/>
       <c r="F78" s="10">
-        <f>ABS(C78-D78)</f>
+        <f t="shared" si="6"/>
         <v>2217.5</v>
       </c>
       <c r="G78" s="11">
-        <f>ABS(C78-E78)</f>
+        <f t="shared" si="7"/>
         <v>2217.5</v>
       </c>
-    </row>
-    <row r="79">
+      <c r="H78" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I78" s="26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
         <v>85</v>
       </c>
@@ -2855,15 +3242,23 @@
       <c r="D79" s="13"/>
       <c r="E79" s="14"/>
       <c r="F79" s="10">
-        <f>ABS(C79-D79)</f>
+        <f t="shared" si="6"/>
         <v>2349.3000000000002</v>
       </c>
       <c r="G79" s="11">
-        <f>ABS(C79-E79)</f>
+        <f t="shared" si="7"/>
         <v>2349.3000000000002</v>
       </c>
-    </row>
-    <row r="80">
+      <c r="H79" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I79" s="26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
         <v>86</v>
       </c>
@@ -2876,15 +3271,23 @@
       <c r="D80" s="13"/>
       <c r="E80" s="14"/>
       <c r="F80" s="10">
-        <f>ABS(C80-D80)</f>
+        <f t="shared" si="6"/>
         <v>2489</v>
       </c>
       <c r="G80" s="11">
-        <f>ABS(C80-E80)</f>
+        <f t="shared" si="7"/>
         <v>2489</v>
       </c>
-    </row>
-    <row r="81">
+      <c r="H80" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I80" s="26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
         <v>87</v>
       </c>
@@ -2897,15 +3300,23 @@
       <c r="D81" s="13"/>
       <c r="E81" s="14"/>
       <c r="F81" s="10">
-        <f>ABS(C81-D81)</f>
+        <f t="shared" si="6"/>
         <v>2637</v>
       </c>
       <c r="G81" s="11">
-        <f>ABS(C81-E81)</f>
+        <f t="shared" si="7"/>
         <v>2637</v>
       </c>
-    </row>
-    <row r="82">
+      <c r="H81" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I81" s="26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
         <v>88</v>
       </c>
@@ -2918,15 +3329,23 @@
       <c r="D82" s="13"/>
       <c r="E82" s="14"/>
       <c r="F82" s="10">
-        <f>ABS(C82-D82)</f>
+        <f t="shared" si="6"/>
         <v>2793</v>
       </c>
       <c r="G82" s="11">
-        <f>ABS(C82-E82)</f>
+        <f t="shared" si="7"/>
         <v>2793</v>
       </c>
-    </row>
-    <row r="83">
+      <c r="H82" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I82" s="26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
         <v>89</v>
       </c>
@@ -2939,15 +3358,23 @@
       <c r="D83" s="13"/>
       <c r="E83" s="14"/>
       <c r="F83" s="10">
-        <f>ABS(C83-D83)</f>
+        <f t="shared" si="6"/>
         <v>2960</v>
       </c>
       <c r="G83" s="11">
-        <f>ABS(C83-E83)</f>
+        <f t="shared" si="7"/>
         <v>2960</v>
       </c>
-    </row>
-    <row r="84">
+      <c r="H83" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I83" s="26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
         <v>90</v>
       </c>
@@ -2960,15 +3387,23 @@
       <c r="D84" s="13"/>
       <c r="E84" s="14"/>
       <c r="F84" s="10">
-        <f>ABS(C84-D84)</f>
+        <f t="shared" si="6"/>
         <v>3136</v>
       </c>
       <c r="G84" s="11">
-        <f>ABS(C84-E84)</f>
+        <f t="shared" si="7"/>
         <v>3136</v>
       </c>
-    </row>
-    <row r="85">
+      <c r="H84" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I84" s="26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
         <v>91</v>
       </c>
@@ -2976,20 +3411,28 @@
         <v>104</v>
       </c>
       <c r="C85" s="13">
-        <v>3222.4000000000001</v>
+        <v>3222.4</v>
       </c>
       <c r="D85" s="13"/>
       <c r="E85" s="14"/>
       <c r="F85" s="10">
-        <f>ABS(C85-D85)</f>
-        <v>3222.4000000000001</v>
+        <f t="shared" si="6"/>
+        <v>3222.4</v>
       </c>
       <c r="G85" s="11">
-        <f>ABS(C85-E85)</f>
-        <v>3222.4000000000001</v>
-      </c>
-    </row>
-    <row r="86">
+        <f t="shared" si="7"/>
+        <v>3222.4</v>
+      </c>
+      <c r="H85" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I85" s="26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
         <v>92</v>
       </c>
@@ -3002,15 +3445,23 @@
       <c r="D86" s="13"/>
       <c r="E86" s="14"/>
       <c r="F86" s="10">
-        <f>ABS(C86-D86)</f>
+        <f t="shared" si="6"/>
         <v>3520</v>
       </c>
       <c r="G86" s="11">
-        <f>ABS(C86-E86)</f>
+        <f t="shared" si="7"/>
         <v>3520</v>
       </c>
-    </row>
-    <row r="87">
+      <c r="H86" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I86" s="26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
         <v>93</v>
       </c>
@@ -3018,20 +3469,28 @@
         <v>106</v>
       </c>
       <c r="C87" s="13">
-        <v>3792.3000000000002</v>
+        <v>3792.3</v>
       </c>
       <c r="D87" s="13"/>
       <c r="E87" s="14"/>
       <c r="F87" s="10">
-        <f>ABS(C87-D87)</f>
-        <v>3792.3000000000002</v>
+        <f t="shared" si="6"/>
+        <v>3792.3</v>
       </c>
       <c r="G87" s="11">
-        <f>ABS(C87-E87)</f>
-        <v>3792.3000000000002</v>
-      </c>
-    </row>
-    <row r="88">
+        <f t="shared" si="7"/>
+        <v>3792.3</v>
+      </c>
+      <c r="H87" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I87" s="26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="s">
         <v>94</v>
       </c>
@@ -3039,44 +3498,58 @@
         <v>107</v>
       </c>
       <c r="C88" s="13">
-        <v>3951.0999999999999</v>
+        <v>3951.1</v>
       </c>
       <c r="D88" s="13"/>
       <c r="E88" s="14"/>
       <c r="F88" s="10">
-        <f>ABS(C88-D88)</f>
-        <v>3951.0999999999999</v>
+        <f t="shared" si="6"/>
+        <v>3951.1</v>
       </c>
       <c r="G88" s="11">
-        <f>ABS(C88-E88)</f>
-        <v>3951.0999999999999</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="17" t="s">
+        <f t="shared" si="7"/>
+        <v>3951.1</v>
+      </c>
+      <c r="H88" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I88" s="26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B89" s="18">
+      <c r="B89" s="17">
         <v>108</v>
       </c>
-      <c r="C89" s="18">
+      <c r="C89" s="17">
         <v>4186</v>
       </c>
-      <c r="D89" s="18"/>
-      <c r="E89" s="19"/>
-      <c r="F89" s="20">
-        <f>ABS(C89-D89)</f>
+      <c r="D89" s="17"/>
+      <c r="E89" s="18"/>
+      <c r="F89" s="19">
+        <f t="shared" si="6"/>
         <v>4186</v>
       </c>
-      <c r="G89" s="21">
-        <f>ABS(C89-E89)</f>
+      <c r="G89" s="20">
+        <f t="shared" si="7"/>
         <v>4186</v>
       </c>
+      <c r="H89" s="23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I89" s="26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
-  <headerFooter/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>